<commit_message>
fixed game fill word
</commit_message>
<xml_diff>
--- a/data/ABSTRACTNOUNS.xlsx
+++ b/data/ABSTRACTNOUNS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TN3Vocab\EnglishTN3Vocab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E33E3A-9C8B-4422-8504-8B7920D48BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FC0FF5-246E-4595-AA4C-F507C1134F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2DF8DC56-1CFA-42D0-9BD6-5FB4458881E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>advice</t>
   </si>
@@ -162,10 +162,528 @@
     <t>Từ vựng / Cụm từ (English)</t>
   </si>
   <si>
-    <t>Nghĩa / Giải thích (Vietnamese/English)</t>
-  </si>
-  <si>
-    <t>Examples</t>
+    <t>Nghĩa / Giải thích (Vietnamese)</t>
+  </si>
+  <si>
+    <t>Examples (Ví dụ)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">She gave me some good </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>advice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> about buying a house.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>crime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> rate in the city has decreased this year.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Education</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is essential for a country's development.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eating vegetables is good for your </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thank you for your </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> with the project.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For more </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, please visit our website.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Buying gold is usually a safe </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>investment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">They are fighting for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>justice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and equality.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>life</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> can be very busy and stressful.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I heard the good </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>news</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> yesterday.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teaching children requires a lot of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>patience</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We all hope for world </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>peace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You are making good </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>progress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in your English studies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do you have any </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>proof</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that you paid the bill?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hard work is the key to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>success</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I don't have enough </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to finish the report.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I have a lot of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>work</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to do this weekend.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">He proposed a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>radical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> change to the company policy.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">She has </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>liberal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> views on social issues.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">He is a politician with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>moderate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> views.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Older generations tend to be more </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>conservative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">His </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>reactionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> opinions were criticized by the public.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -181,17 +699,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,13 +747,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,17 +1072,17 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -574,205 +1093,250 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>